<commit_message>
Evaluate circuit depth vs. accuracy
</commit_message>
<xml_diff>
--- a/spreadsheets/BSE16qubit_mean_encoder.xlsx
+++ b/spreadsheets/BSE16qubit_mean_encoder.xlsx
@@ -485,7 +485,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.7261509110052228</v>
+        <v>0.7261509110052229</v>
       </c>
     </row>
     <row r="7">
@@ -535,7 +535,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.04688115307313915</v>
+        <v>0.04688115307313914</v>
       </c>
     </row>
     <row r="12">
@@ -565,7 +565,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.527506874197718</v>
+        <v>0.5275068741977181</v>
       </c>
     </row>
     <row r="15">

</xml_diff>

<commit_message>
Tue  5 Nov 2024 15:36:34 EST
</commit_message>
<xml_diff>
--- a/spreadsheets/BSE16qubit_mean_encoder.xlsx
+++ b/spreadsheets/BSE16qubit_mean_encoder.xlsx
@@ -445,7 +445,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.5483334058394633</v>
+        <v>-0.5132311925419113</v>
       </c>
     </row>
     <row r="3">
@@ -455,7 +455,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.4388152899725492</v>
+        <v>-0.2443230223947546</v>
       </c>
     </row>
     <row r="4">
@@ -465,7 +465,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2924055799924064</v>
+        <v>-0.1122969665579973</v>
       </c>
     </row>
     <row r="5">
@@ -475,7 +475,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.2633722774678172</v>
+        <v>-0.6735928914736183</v>
       </c>
     </row>
     <row r="6">
@@ -485,7 +485,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.7261509110052229</v>
+        <v>-0.5828406572137433</v>
       </c>
     </row>
     <row r="7">
@@ -495,7 +495,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.5856228053907445</v>
+        <v>-0.5581692505993664</v>
       </c>
     </row>
     <row r="8">
@@ -505,7 +505,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.5279640510362523</v>
+        <v>-0.1294327888515099</v>
       </c>
     </row>
     <row r="9">
@@ -515,7 +515,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.4028384916812342</v>
+        <v>-0.1767356733746669</v>
       </c>
     </row>
     <row r="10">
@@ -525,7 +525,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.3070763867582285</v>
+        <v>-0.2001013470520436</v>
       </c>
     </row>
     <row r="11">
@@ -535,7 +535,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.04688115307313914</v>
+        <v>-0.3985823049844313</v>
       </c>
     </row>
     <row r="12">
@@ -545,7 +545,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.6404433048987681</v>
+        <v>-0.3336059981250021</v>
       </c>
     </row>
     <row r="13">
@@ -555,7 +555,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.5512165644000019</v>
+        <v>-0.1885847338511432</v>
       </c>
     </row>
     <row r="14">
@@ -565,7 +565,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.5275068741977181</v>
+        <v>-0.1726523228640892</v>
       </c>
     </row>
     <row r="15">
@@ -575,7 +575,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.3362693909433243</v>
+        <v>0.01729299512457281</v>
       </c>
     </row>
   </sheetData>

</xml_diff>